<commit_message>
Ajout GCI et Prédiction
</commit_message>
<xml_diff>
--- a/resultatpourgci.xlsx
+++ b/resultatpourgci.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucka\Documents\École\mec8211\Final_projet_mec8211\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97A192E-888B-4D90-82E9-A6DA33DD5B34}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BB04E7-CEB8-47EE-B023-020DC9DE4432}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00A33AFD-4C72-41CB-86B4-5AE67C4E076A}"/>
   </bookViews>
@@ -514,6 +514,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="659463615"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
@@ -617,6 +618,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="659902527"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
@@ -679,6 +681,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="659464031"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2721,8 +2724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0524374-FEBB-4EC6-A6E9-2E497850F45F}">
   <dimension ref="C1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>